<commit_message>
LapNV: integrate notifications code
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_Driver_v0.4.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_Driver_v0.4.xlsx
@@ -4,40 +4,44 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="18"/>
+    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010" tabRatio="875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="4" r:id="rId1"/>
-    <sheet name="UpdateCurrentLocation" sheetId="20" r:id="rId2"/>
-    <sheet name="UpdateDriverStatus" sheetId="26" r:id="rId3"/>
-    <sheet name="UpdateAddress" sheetId="27" r:id="rId4"/>
-    <sheet name="Update Driver Info" sheetId="5" r:id="rId5"/>
-    <sheet name="Change Password" sheetId="6" r:id="rId6"/>
-    <sheet name="Get List Vip Riders" sheetId="9" r:id="rId7"/>
-    <sheet name="DeleteVipRider" sheetId="28" r:id="rId8"/>
-    <sheet name="Add Vip Rider" sheetId="12" r:id="rId9"/>
-    <sheet name="GetRiderImage" sheetId="30" r:id="rId10"/>
-    <sheet name="AcceptTrip" sheetId="21" r:id="rId11"/>
-    <sheet name="RejectTrip" sheetId="22" r:id="rId12"/>
-    <sheet name="CancelTrip" sheetId="24" r:id="rId13"/>
-    <sheet name="StartTrip" sheetId="23" r:id="rId14"/>
-    <sheet name="CompleteTrip" sheetId="25" r:id="rId15"/>
-    <sheet name="Get My Trips" sheetId="10" r:id="rId16"/>
-    <sheet name="Register Promotion Trip" sheetId="15" r:id="rId17"/>
-    <sheet name="MyPromotionTrips" sheetId="29" r:id="rId18"/>
-    <sheet name="UpdatePromotionTrip" sheetId="16" r:id="rId19"/>
-    <sheet name="Sheet6" sheetId="31" r:id="rId20"/>
+    <sheet name="selectAvailableVehicle" sheetId="34" r:id="rId2"/>
+    <sheet name="UpdateCurrentLocation" sheetId="20" r:id="rId3"/>
+    <sheet name="UpdateDriverStatus" sheetId="26" r:id="rId4"/>
+    <sheet name="UpdateAddress" sheetId="27" r:id="rId5"/>
+    <sheet name="Update Driver Info" sheetId="5" r:id="rId6"/>
+    <sheet name="Change Password" sheetId="6" r:id="rId7"/>
+    <sheet name="Get List Vip Riders" sheetId="9" r:id="rId8"/>
+    <sheet name="DeleteVipRider" sheetId="28" r:id="rId9"/>
+    <sheet name="Add Vip Rider" sheetId="12" r:id="rId10"/>
+    <sheet name="GetRiderImage" sheetId="30" r:id="rId11"/>
+    <sheet name="AcceptTrip" sheetId="21" r:id="rId12"/>
+    <sheet name="RejectTrip" sheetId="22" r:id="rId13"/>
+    <sheet name="CancelTrip" sheetId="24" r:id="rId14"/>
+    <sheet name="StartTrip" sheetId="23" r:id="rId15"/>
+    <sheet name="CompleteTrip" sheetId="25" r:id="rId16"/>
+    <sheet name="Get My Trips" sheetId="10" r:id="rId17"/>
+    <sheet name="Register Promotion Trip" sheetId="15" r:id="rId18"/>
+    <sheet name="MyPromotionTrips" sheetId="29" r:id="rId19"/>
+    <sheet name="UpdatePromotionTrip" sheetId="16" r:id="rId20"/>
+    <sheet name="Sheet6" sheetId="31" r:id="rId21"/>
+    <sheet name="Sheet1" sheetId="32" r:id="rId22"/>
+    <sheet name="Sheet2" sheetId="33" r:id="rId23"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="246">
   <si>
     <t>String</t>
   </si>
@@ -717,13 +721,73 @@
   </si>
   <si>
     <t>/CommonController</t>
+  </si>
+  <si>
+    <t>selectAvailableVehice</t>
+  </si>
+  <si>
+    <t>oPrice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oKm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f1Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f1Km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f2Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f2Km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f3Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f3Km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">f4Price </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vehicleId </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">carTitle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">carLevel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">manuYear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t>vehicleInfos</t>
+  </si>
+  <si>
+    <t>Doube?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f4Km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vRegDate </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,6 +847,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF373E4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1060,7 +1130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1190,6 +1260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1220,6 +1291,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1555,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,6 +2179,157 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="67.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="102" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="103"/>
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="103"/>
+      <c r="B5" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="103"/>
+      <c r="B6" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="103"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="51"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="104"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="103"/>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="103"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="105"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
@@ -2139,7 +2374,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="102" t="s">
         <v>118</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -2153,7 +2388,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="102"/>
+      <c r="A4" s="103"/>
       <c r="B4" s="6" t="s">
         <v>43</v>
       </c>
@@ -2165,7 +2400,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="102"/>
+      <c r="A5" s="103"/>
       <c r="B5" s="7" t="s">
         <v>44</v>
       </c>
@@ -2177,7 +2412,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
+      <c r="A6" s="103"/>
       <c r="B6" s="53" t="s">
         <v>59</v>
       </c>
@@ -2187,19 +2422,19 @@
       <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="102"/>
+      <c r="A7" s="103"/>
       <c r="B7" s="53"/>
       <c r="C7" s="52"/>
       <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
+      <c r="A8" s="104"/>
       <c r="B8" s="13"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="102" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -2213,7 +2448,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="102"/>
+      <c r="A10" s="103"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2458,7 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="102"/>
+      <c r="A11" s="103"/>
       <c r="B11" s="6" t="s">
         <v>16</v>
       </c>
@@ -2231,7 +2466,7 @@
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="102"/>
+      <c r="A12" s="103"/>
       <c r="B12" s="7" t="s">
         <v>19</v>
       </c>
@@ -2239,7 +2474,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="102"/>
+      <c r="A13" s="103"/>
       <c r="B13" s="7" t="s">
         <v>198</v>
       </c>
@@ -2249,7 +2484,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104"/>
+      <c r="A14" s="105"/>
       <c r="B14" s="3" t="s">
         <v>197</v>
       </c>
@@ -2267,12 +2502,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,12 +2739,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,12 +2971,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2970,12 +3205,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3208,12 +3443,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,7 +3701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
@@ -3789,7 +4024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -4061,7 +4296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
@@ -4500,11 +4735,355 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="95" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="43"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="43"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="D20" s="34"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="106" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="B22" s="107" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="34"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="107" t="s">
+        <v>229</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="D23" s="34"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39"/>
+      <c r="B24" s="106" t="s">
+        <v>230</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="D24" s="42"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="107" t="s">
+        <v>231</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="108" t="s">
+        <v>232</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="107" t="s">
+        <v>233</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="109" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="108" t="s">
+        <v>235</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="108" t="s">
+        <v>244</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="108" t="s">
+        <v>236</v>
+      </c>
+      <c r="C31" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="108" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="108" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="108" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="108" t="s">
+        <v>245</v>
+      </c>
+      <c r="C35" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="108" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="108" t="s">
+        <v>241</v>
+      </c>
+      <c r="C37" s="110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -4710,229 +5289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="42.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="34"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="34"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="34"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="34"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="34"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="34"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="43"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="43"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="37"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="34"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="37"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="37"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="39"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
@@ -5132,12 +5489,258 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
+      <c r="B6" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
+      <c r="B7" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="34"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="34"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="43"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="43"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="37"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="37"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="34"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="37"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="34"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="37"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="34"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="34"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5320,7 +5923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -5537,7 +6140,7 @@
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="95" t="s">
+      <c r="A21" s="96" t="s">
         <v>93</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -5551,19 +6154,19 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
+      <c r="A22" s="97"/>
       <c r="B22" s="56"/>
       <c r="C22" s="55"/>
       <c r="D22" s="54"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="96"/>
+      <c r="A23" s="97"/>
       <c r="B23" s="53"/>
       <c r="C23" s="52"/>
       <c r="D23" s="51"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
+      <c r="A24" s="97"/>
       <c r="B24" s="53" t="s">
         <v>14</v>
       </c>
@@ -5575,19 +6178,19 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="96"/>
+      <c r="A25" s="97"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
+      <c r="A26" s="97"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="97"/>
+      <c r="A27" s="98"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
@@ -5600,7 +6203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -5890,7 +6493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -6109,7 +6712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
@@ -6154,7 +6757,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="98" t="s">
+      <c r="A3" s="99" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -6168,7 +6771,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
+      <c r="A4" s="100"/>
       <c r="B4" s="6" t="s">
         <v>23</v>
       </c>
@@ -6178,7 +6781,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
+      <c r="A5" s="100"/>
       <c r="B5" s="53" t="s">
         <v>107</v>
       </c>
@@ -6190,19 +6793,19 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
+      <c r="A6" s="100"/>
       <c r="B6" s="53"/>
       <c r="C6" s="52"/>
       <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="99"/>
+      <c r="A7" s="100"/>
       <c r="B7" s="53"/>
       <c r="C7" s="52"/>
       <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="100"/>
+      <c r="A8" s="101"/>
       <c r="B8" s="13"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
@@ -6319,7 +6922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -6464,155 +7067,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="67.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
-        <v>118</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="102"/>
-      <c r="B4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="102"/>
-      <c r="B5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="102"/>
-      <c r="B6" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="102"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="51"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="102"/>
-      <c r="B10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="102"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="104"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A8"/>
-    <mergeCell ref="A9:A12"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
LapNV: Update Car icon and Process Bar
Signed-off-by: apolong <apolong.lap@gmail.com>
</commit_message>
<xml_diff>
--- a/WIP/Documents/TNET_WebServiceDesign_Driver_v0.4.xlsx
+++ b/WIP/Documents/TNET_WebServiceDesign_Driver_v0.4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010" tabRatio="875" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010" tabRatio="875"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="247">
   <si>
     <t>String</t>
   </si>
@@ -780,6 +780,9 @@
   </si>
   <si>
     <t xml:space="preserve">vRegDate </t>
+  </si>
+  <si>
+    <t>Cái này để lấy danh sách xe hợp lệ</t>
   </si>
 </sst>
 </file>
@@ -1638,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4739,7 +4742,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4820,7 +4823,9 @@
       <c r="C6" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="34" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="28"/>
@@ -5738,7 +5743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>